<commit_message>
naamgeving aangepast, excel read aangepast
</commit_message>
<xml_diff>
--- a/Assignment2/code/AirportData.xlsx
+++ b/Assignment2/code/AirportData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fos van der Meer\Documents\Uni\TIL\AE4423\Assignments\AE4423\Assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fos van der Meer\Documents\Uni\TIL\AE4423\Assignments\AE4423\Assignment2\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CA2363-EFE5-458A-8637-718B1BAB3985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E9C7232-2EC2-48FA-A412-3C0BD9AE1664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8F9EF160-6BC0-D24A-9525-A45551C45E1F}"/>
   </bookViews>
@@ -568,7 +568,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>